<commit_message>
MapNpc id 칼럼 수정
</commit_message>
<xml_diff>
--- a/excel/MapNpcData.xlsx
+++ b/excel/MapNpcData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD4FA77-9EA3-0446-8FE5-86CB4ED39290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB78BBF-D0D7-7441-9971-6C9D361A01DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="680" windowWidth="29400" windowHeight="16520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MapNpcInfoData" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
-  <si>
-    <t>int;key</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>NpcId</t>
   </si>
@@ -101,6 +97,14 @@
   </si>
   <si>
     <t>Talk</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>int;id</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>int;id;key</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -476,8 +480,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -490,37 +494,37 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>3</v>
       </c>
       <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:6" ht="15">
       <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>7</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -550,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86050EB-D00F-8A40-897C-29FC87B050D7}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -564,70 +568,70 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="D2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15">
       <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>7</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15">
       <c r="A4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>7</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MapNpcData에 list 칼럼 추가
</commit_message>
<xml_diff>
--- a/excel/MapNpcData.xlsx
+++ b/excel/MapNpcData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB78BBF-D0D7-7441-9971-6C9D361A01DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3F09C0-D3C1-B04E-BF68-62F5EB11C7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>NpcId</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>int;id;key</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>list&lt;int&gt;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShowRequirementValue</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>HideRequirementValue</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -239,12 +251,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -255,7 +264,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -478,71 +486,402 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="4"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="12"/>
+    <col min="1" max="1" width="12.5" style="3"/>
+    <col min="2" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A2" s="10" t="s">
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="11"/>
-    </row>
-    <row r="3" spans="1:6" ht="15">
-      <c r="A3" s="8" t="s">
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" ht="15">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" ht="15">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-    </row>
-    <row r="6" spans="1:6" ht="13"/>
-    <row r="7" spans="1:6" ht="13"/>
-    <row r="12" spans="1:6" ht="13">
-      <c r="F12" s="1"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="15">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="15">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="13">
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="13">
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" customHeight="1">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" customHeight="1">
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" customHeight="1">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="13">
+      <c r="E12" s="2"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" customHeight="1">
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" customHeight="1">
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" customHeight="1">
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" customHeight="1">
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E25" s="2"/>
+    </row>
+    <row r="26" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E77" s="2"/>
+    </row>
+    <row r="78" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E79" s="2"/>
+    </row>
+    <row r="80" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E86" s="2"/>
+    </row>
+    <row r="87" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E88" s="2"/>
+    </row>
+    <row r="89" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E89" s="2"/>
+    </row>
+    <row r="90" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E90" s="2"/>
+    </row>
+    <row r="91" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E91" s="2"/>
+    </row>
+    <row r="92" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E93" s="2"/>
+    </row>
+    <row r="94" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E94" s="2"/>
+    </row>
+    <row r="95" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E95" s="2"/>
+    </row>
+    <row r="96" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E96" s="2"/>
+    </row>
+    <row r="97" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E97" s="2"/>
+    </row>
+    <row r="98" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E98" s="2"/>
+    </row>
+    <row r="99" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E99" s="2"/>
+    </row>
+    <row r="100" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E100" s="2"/>
+    </row>
+    <row r="101" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E101" s="2"/>
+    </row>
+    <row r="102" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E102" s="2"/>
+    </row>
+    <row r="103" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E103" s="2"/>
+    </row>
+    <row r="104" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E104" s="2"/>
+    </row>
+    <row r="105" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E105" s="2"/>
+    </row>
+    <row r="106" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E106" s="2"/>
+    </row>
+    <row r="107" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E107" s="2"/>
+    </row>
+    <row r="108" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E108" s="2"/>
+    </row>
+    <row r="109" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E109" s="2"/>
+    </row>
+    <row r="110" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E110" s="2"/>
+    </row>
+    <row r="111" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E111" s="2"/>
+    </row>
+    <row r="112" spans="5:5" ht="15.75" customHeight="1">
+      <c r="E112" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -567,70 +906,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MapNpcData에 list 칼럼 추가2
</commit_message>
<xml_diff>
--- a/excel/MapNpcData.xlsx
+++ b/excel/MapNpcData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3F09C0-D3C1-B04E-BF68-62F5EB11C7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4325950-59ED-1949-A992-A4B5DB4A7A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>NpcId</t>
   </si>
@@ -112,11 +112,11 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>ShowRequirementValue</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>HideRequirementValue</t>
+    <t>HideRequirementValues</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShowRequirementValues</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -489,7 +489,7 @@
   <dimension ref="A1:G112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -525,13 +525,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15">
@@ -891,21 +891,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86050EB-D00F-8A40-897C-29FC87B050D7}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="2" max="3" width="24" customWidth="1"/>
+    <col min="4" max="5" width="21" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -913,63 +913,79 @@
         <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="E3" s="9"/>
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15">
+    <row r="4" spans="1:7" ht="15">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4">
+      <c r="E4" s="9"/>
+      <c r="F4">
         <v>2</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Npc] CompassUI를 위한 데이터 추가2
</commit_message>
<xml_diff>
--- a/excel/MapNpcData.xlsx
+++ b/excel/MapNpcData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F7FA2E-2CF5-5049-9A75-48F31E02BDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA45A32-E94E-7B41-BF6C-13E9476555F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="900" windowWidth="27780" windowHeight="15620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>NpcId</t>
   </si>
@@ -298,6 +298,10 @@
   </si>
   <si>
     <t>ShowBubble</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Priority</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1123,10 +1127,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86050EB-D00F-8A40-897C-29FC87B050D7}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1136,10 +1140,10 @@
     <col min="3" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
     <col min="6" max="6" width="27.1640625" customWidth="1"/>
-    <col min="9" max="10" width="25.6640625" customWidth="1"/>
+    <col min="10" max="11" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="15" customFormat="1">
+    <row r="1" spans="1:11" s="15" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>10</v>
       </c>
@@ -1162,16 +1166,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="15" customFormat="1">
+    <row r="2" spans="1:11" s="15" customFormat="1">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
@@ -1194,16 +1201,19 @@
         <v>7</v>
       </c>
       <c r="H2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:11" ht="15">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1220,16 +1230,19 @@
         <v>1</v>
       </c>
       <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>0</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:11" ht="15">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1246,9 +1259,12 @@
         <v>2</v>
       </c>
       <c r="H4">
+        <v>10</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
npc position data 수정
</commit_message>
<xml_diff>
--- a/excel/MapNpcData.xlsx
+++ b/excel/MapNpcData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7AABAC-9327-B14E-9DC2-6BE62328DFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DBB395-0650-8548-A057-EA35AD2AE3FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="27420" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="27420" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MapNpcInfo" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>NpcId</t>
   </si>
@@ -500,9 +500,6 @@
   <si>
     <t>ShowMenuPopup</t>
     <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>int;id;key</t>
   </si>
   <si>
     <r>
@@ -1014,13 +1011,13 @@
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
@@ -1031,13 +1028,13 @@
         <v>22</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15">
@@ -1048,7 +1045,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1065,13 +1062,13 @@
         <v>26</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15">
@@ -1082,13 +1079,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="13"/>
@@ -1105,8 +1102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C46EA2E-F947-224D-A4BE-A46A7E528B7A}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1119,7 +1116,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="18" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
@@ -1128,10 +1125,10 @@
         <v>10</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1145,25 +1142,25 @@
         <v>11</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15">
       <c r="A3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15">
@@ -1185,7 +1182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86050EB-D00F-8A40-897C-29FC87B050D7}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
[Map] npc 데이터 수정2
</commit_message>
<xml_diff>
--- a/excel/MapNpcData.xlsx
+++ b/excel/MapNpcData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE446D7-8E2A-1A46-A4CC-5060AE02B67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20DAC68-96F5-4647-B798-7FB508A33ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="1160" windowWidth="21560" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="3540" windowWidth="22000" windowHeight="12220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MapNpcInfo" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>NpcId</t>
   </si>
@@ -561,10 +561,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>0,0,0.5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>-21,248</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -648,6 +644,21 @@
   </si>
   <si>
     <t>-381,6</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResourceKey</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>img_powder_shop_mirror</t>
+  </si>
+  <si>
+    <t>0,36,0.5</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -815,7 +826,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -851,6 +862,10 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1069,80 +1084,88 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.83203125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="20"/>
-    <col min="5" max="5" width="17.33203125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="20"/>
+    <col min="6" max="6" width="17.33203125" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="E2" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="F2" s="19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="20">
+      <c r="C3" s="6"/>
+      <c r="D3" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="20">
         <v>40</v>
       </c>
-      <c r="E3" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15">
+      <c r="F3" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15">
       <c r="A4" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>48</v>
+      <c r="C4" t="s">
+        <v>58</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>47</v>
@@ -1150,27 +1173,31 @@
       <c r="E4" s="19" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15">
+      <c r="F4" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>54</v>
-      </c>
+      <c r="C5" s="16"/>
       <c r="D5" s="19" t="s">
         <v>53</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="13"/>
-    <row r="11" spans="1:5" ht="13">
-      <c r="C11" s="21"/>
+        <v>52</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="13"/>
+    <row r="11" spans="1:6" ht="13">
+      <c r="D11" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1182,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C46EA2E-F947-224D-A4BE-A46A7E528B7A}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1246,17 +1273,17 @@
     </row>
     <row r="4" spans="1:5" ht="15">
       <c r="A4" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>50</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15">
@@ -1267,10 +1294,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1284,7 +1311,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:H5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
[Map] npc 데이터 수정3
</commit_message>
<xml_diff>
--- a/excel/MapNpcData.xlsx
+++ b/excel/MapNpcData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A20DAC68-96F5-4647-B798-7FB508A33ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82548223-FBA7-534E-AEE6-47F22C3E1DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="3540" windowWidth="22000" windowHeight="12220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="3540" windowWidth="22000" windowHeight="12220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MapNpcInfo" sheetId="1" r:id="rId1"/>
@@ -545,10 +545,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>ColliderScale</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>CompassUIPosition</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -659,6 +655,10 @@
   </si>
   <si>
     <t>0,36,0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ColliderRadius</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -862,10 +862,10 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1087,7 +1087,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1107,16 +1107,16 @@
         <v>4</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>40</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
@@ -1127,16 +1127,16 @@
         <v>22</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>41</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15">
@@ -1148,13 +1148,13 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="20">
         <v>40</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15">
@@ -1165,16 +1165,16 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15">
@@ -1186,13 +1186,13 @@
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>53</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13"/>
@@ -1209,7 +1209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C46EA2E-F947-224D-A4BE-A46A7E528B7A}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1236,7 +1236,7 @@
         <v>35</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1268,22 +1268,22 @@
         <v>38</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15">
       <c r="A4" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>49</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15">
@@ -1294,10 +1294,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86050EB-D00F-8A40-897C-29FC87B050D7}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
[Map] npc object info 시트 추가
</commit_message>
<xml_diff>
--- a/excel/MapNpcData.xlsx
+++ b/excel/MapNpcData.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82548223-FBA7-534E-AEE6-47F22C3E1DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5401BBAC-512F-9F48-BB45-CA3D903366EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="3540" windowWidth="22000" windowHeight="12220" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="3540" windowWidth="22000" windowHeight="12220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MapNpcInfo" sheetId="1" r:id="rId1"/>
-    <sheet name="MapNpcPosition" sheetId="3" r:id="rId2"/>
-    <sheet name="MapNpcMenu" sheetId="2" r:id="rId3"/>
+    <sheet name="MapObjectInfo" sheetId="4" r:id="rId2"/>
+    <sheet name="MapNpcPosition" sheetId="3" r:id="rId3"/>
+    <sheet name="MapNpcMenu" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>NpcId</t>
   </si>
@@ -623,10 +624,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>0,220</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>150</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -659,6 +656,10 @@
   </si>
   <si>
     <t>ColliderRadius</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,145</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1084,10 +1085,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1107,7 +1108,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
@@ -1127,13 +1128,13 @@
         <v>22</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F2" s="19" t="s">
         <v>41</v>
@@ -1148,56 +1149,36 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="20">
         <v>40</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15">
       <c r="A4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="16"/>
       <c r="D4" s="19" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15">
-      <c r="A5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="13"/>
-    <row r="11" spans="1:6" ht="13">
-      <c r="D11" s="21"/>
+    </row>
+    <row r="5" spans="1:6" ht="13"/>
+    <row r="10" spans="1:6" ht="13">
+      <c r="D10" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1206,11 +1187,84 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8734686-E2F1-F449-89E3-311F262D7FCD}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C46EA2E-F947-224D-A4BE-A46A7E528B7A}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1297,7 +1351,7 @@
         <v>48</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1306,12 +1360,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86050EB-D00F-8A40-897C-29FC87B050D7}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
static npc menu data 추가
</commit_message>
<xml_diff>
--- a/excel/MapNpcData.xlsx
+++ b/excel/MapNpcData.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geugkkom/Documents/Tsomsomm/lunaria-data/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E524E2A2-E323-084C-AE29-D8D4948E7D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82AD649-F15F-FE40-BACF-48F6A04B773D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="3540" windowWidth="22000" windowHeight="12220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MapNpcInfo" sheetId="1" r:id="rId1"/>
-    <sheet name="MapStaticNpcInfo" sheetId="4" r:id="rId2"/>
-    <sheet name="MapNpcPosition" sheetId="3" r:id="rId3"/>
-    <sheet name="MapNpcMenu" sheetId="2" r:id="rId4"/>
+    <sheet name="MapNpcPosition" sheetId="3" r:id="rId2"/>
+    <sheet name="MapNpcMenu" sheetId="2" r:id="rId3"/>
+    <sheet name="MapStaticNpcMenu" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>NpcId</t>
   </si>
@@ -401,6 +401,17 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <t>PlayPowderPortalMinigame</t>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ShowMenuPopup</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <t>[</t>
     </r>
@@ -412,7 +423,123 @@
         <family val="2"/>
         <charset val="129"/>
       </rPr>
-      <t>파우더상점</t>
+      <t>마이홈_슬라임]</t>
+    </r>
+  </si>
+  <si>
+    <t>MyhomeSlimeAppeared</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>enum&lt;MapType&gt;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>MapType</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Positions</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Myhome</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpritePositionAndScale</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>CompassUIPosition</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>list&lt;float&gt;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>343,-28.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>PowderShop</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>150</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,78,0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,280</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>-381,6</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,36,0.5</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>ColliderRadius</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,145</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>int;id</t>
+  </si>
+  <si>
+    <t>local_string;[NpcId][Order]</t>
+  </si>
+  <si>
+    <t>enum&lt;RequirementType&gt;</t>
+  </si>
+  <si>
+    <t>list&lt;int&gt;</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>enum&lt;NpcMenuFunctionType&gt;</t>
+  </si>
+  <si>
+    <t>MenuName</t>
+  </si>
+  <si>
+    <t>ShowRequirement</t>
+  </si>
+  <si>
+    <t>ShowRequirementValues</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>FunctionType</t>
+  </si>
+  <si>
+    <t>FunctionValue</t>
+  </si>
+  <si>
+    <t>AlwaysTrue</t>
+  </si>
+  <si>
+    <r>
+      <t>미니게임</t>
     </r>
     <r>
       <rPr>
@@ -420,8 +547,9 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
-      </rPr>
-      <t>_</t>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -431,243 +559,18 @@
         <family val="2"/>
         <charset val="129"/>
       </rPr>
-      <t>거울</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>파우더상점</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>거울</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]</t>
-    </r>
-  </si>
-  <si>
-    <t>PlayPowderPortalMinigame</t>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ShowMenuPopup</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>마이홈_슬라임]</t>
-    </r>
-  </si>
-  <si>
-    <t>MyhomeSlimeAppeared</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>enum&lt;MapType&gt;</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>MapType</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Positions</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Myhome</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>SpritePositionAndScale</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>float</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>CompassUIPosition</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>list&lt;float&gt;</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>343,-28.5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>-21,248</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>50</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>-22,84,1</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>파우더상점</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Malgun Gothic"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>거울</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>PowderShop</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>-195,21</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>150</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,78,0.5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,280</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>-381,6</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ResourceKey</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>img_powder_shop_mirror</t>
-  </si>
-  <si>
-    <t>0,36,0.5</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>ColliderRadius</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>0,145</t>
-    <phoneticPr fontId="4" type="noConversion"/>
+      <t>시작</t>
+    </r>
+  </si>
+  <si>
+    <t>[파우더상점_거울]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -741,8 +644,15 @@
       <name val="Roboto"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -779,8 +689,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FFEFEFEF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBFBFBF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -823,11 +745,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD9D9D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD9D9D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD9D9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD9D9D9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD9D9D9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFD9D9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD9D9D9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFD9D9D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -863,10 +822,19 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1085,100 +1053,91 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="20"/>
-    <col min="6" max="6" width="17.33203125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="20"/>
+    <col min="5" max="5" width="17.33203125" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>54</v>
+      <c r="C1" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>55</v>
+      <c r="C2" s="19" t="s">
+        <v>37</v>
       </c>
       <c r="D2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15">
+    </row>
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="20">
+      <c r="C3" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="20">
         <v>40</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15">
+      <c r="E3" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="19" t="s">
+        <v>44</v>
+      </c>
       <c r="D4" s="19" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="13"/>
-    <row r="10" spans="1:6" ht="13">
-      <c r="D10" s="21"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="13"/>
+    <row r="10" spans="1:5" ht="13">
+      <c r="C10" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1187,85 +1146,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8734686-E2F1-F449-89E3-311F262D7FCD}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C46EA2E-F947-224D-A4BE-A46A7E528B7A}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15">
-      <c r="A3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C46EA2E-F947-224D-A4BE-A46A7E528B7A}">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1288,10 +1173,10 @@
         <v>10</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1305,54 +1190,39 @@
         <v>11</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15">
       <c r="A3" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15">
       <c r="A4" s="18" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5"/>
       <c r="D4" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15">
-      <c r="A5" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1361,12 +1231,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86050EB-D00F-8A40-897C-29FC87B050D7}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1398,7 +1268,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>7</v>
@@ -1427,7 +1297,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>6</v>
@@ -1511,28 +1381,103 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6">
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34C47EBB-6A27-BC46-836F-0B164FBA73C0}">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="25.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15">
+      <c r="A3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="F3" s="6">
         <v>1</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
+      <c r="G3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>